<commit_message>
19.8.19 stagged changes from before
</commit_message>
<xml_diff>
--- a/project_work/tossembler_outerloops.xlsx
+++ b/project_work/tossembler_outerloops.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\nayah\Documents\cpuC-Project\project_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CF0166-3AE0-4395-8139-2BE205D09A0D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA29207-028D-46CD-9955-3FD9C5D54790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>R1 = r</t>
   </si>
@@ -66,21 +66,6 @@
     <t>C12 = end of loop 3.2 (with n the elements in row m)</t>
   </si>
   <si>
-    <t xml:space="preserve">     PC=PC+1 || R2=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Mux(PC+1, PC+C12, R3&lt;C2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        R3=R3+1 || PC=C16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R2=R2+1 || PC=C14</t>
-  </si>
-  <si>
-    <t>R1=R1+1 || PC = C13</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -192,50 +177,6 @@
     <t>C23 = 6</t>
   </si>
   <si>
-    <t>PC=PC+1 || R1=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        PC=PC+1 || R11 = R5+R6+R7+R8+R9+R10 || R3=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        PC=PC+1 || R1` = R2*C2+C1/*R1`=R3`+C1*/ || R2` = R1*C8-1/*R2`=R1`-1*/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    PC=PC+1 || y[R1*C6+R2*C2+R3] += R11 || R11 = R11-R5+R4 || R5=R6|| R6=R7|| R7=R8|| R8=R9|| R9=R10|| R10=R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    PC=PC+1 || R4 =  (Rout0in_layer*Rout0weight + Rout1in_layer*Rout1weight + Rout2in_layer*Rout2weight) +
-                    (Rout3in_layer*Rout3weight + Rout4in_layer*Rout4weight + Rout5in_layer*Rout5weight) || R1` = R1`+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          PC=PC+1 || R3=0 || R1` = R2*C2 || R2` = R1*C8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        R2`=R2`+1 || R1`=R1`+1 || R3=R3+1 || PC=C15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               R5 = Mux(R4, R5, R3==0) || R6 = Mux(R4, R6, R3==1) || R7 = Mux(R4, R7, R3==2) ||  R8 = Mux(R4, R8, R3==3) ||  R9 = Mux(R4, R9, R3==4) || R10 = Mux(R4, R10, R3==5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               PC=PC+1 ||
-               R4 = (Rout0in_layer*Rout0weight + Rout1in_layer*Rout1weight + Rout2in_layer*Rout2weight) +  (Rout3in_layer*Rout3weight + Rout4in_layer*Rout4weight + Rout5in_layer*Rout5weight)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               PC=PC+1 ||
-               Radd0in_layer = R1` || Radd1in_layer = R1`+C2 || Radd2in_layer = R1`+2*C2 || Radd3in_layer = R1`+3*C2 || Radd4in_layer = R1`+4*C2 || Radd5in_layer = R1`+5*C2 ||
-               Radd0weight   = R2` || Radd1weight   = R2`+C1 || Radd2weight   = R2`+2*C1 || Radd3weight   = R2`+3*C1 || Radd4weight   = R2`+4*C1 || Radd5weight   = R2`+5*C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        PC=PC+1 ||
-        Radd0in_layer = R1` || Radd1in_layer = R1`+C2 || Radd2in_layer = R1`+2*C2 || Radd3in_layer = R1`+3*C2 || Radd4in_layer = R1`+4*C2 || Radd5in_layer = R1`+5*C2 ||
-        Radd0weight   = R2`+C1 || Radd1weight   = R2`+2*C1 || Radd2weight   = R2`+3*C1 || Radd3weight   = R2`+4*C1 || Radd4weight   = R2`+5*C1 || Radd5weight   = R2`+6*C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    PC=PC+1 ||
-                    Radd0in_layer = R1` || Radd1in_layer = R1`+C2 || Radd2in_layer = R1`+2*C2 || Radd3in_layer = R1`+3*C2 || Radd4in_layer = R1`+4*C2 || Radd5in_layer = R1`+5*C2 ||
-                    Radd0weight   = R2`+C1 || Radd1weight   = R2`+2*C1 || Radd2weight   = R2`+3*C1 || Radd3weight   = R2`+4*C1 || Radd4weight   = R2`+5*C1 || Radd5weight   = R2`+6*C1</t>
-  </si>
-  <si>
     <t>R20-R25</t>
   </si>
   <si>
@@ -246,6 +187,54 @@
   </si>
   <si>
     <t>constants = 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     PC=PC+1 || R2=0 || R20=0 || R21=C2 || R22=2*C2 || R23=3*C2 || R24=4*C2 || R25=5*C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               PC=PC+1 || A0I  = R20 || A1I  = R21 || A2I  = R22 || A3I  = R23 || A4I  = R24 || A5I  = R25 || A0W  = R30 || A1W  = R31 || A2W  = R32 || A3W  = R33 || A4W  = R34 || A5W  = R35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               PC=PC+1 ||  R4 = M0I*M0W + M1I*M1W + M2I*M2W + M3I*M3W + M4I*M4W + M5I*M5W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        PC=PC+1 || R11 = R5+R6+R7+R8+R9+R10 || R3=0 || A0I = R20 || A1I = R21 || A2I = R22 || A3I = R23 || A4I = R24 || A5I = R25 || A0W = R30-=1 || A1W = R31-=1 || A2W = R32-=1 || A3W = R33-=1 || A4W = R34-=1 || A5W = R35-=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R2=R2+1 || PC=C14 || R20-=C1 || R21-=C1 || R22-=C1 || R23-=C1 || R24-=C1 || R25-=C1</t>
+  </si>
+  <si>
+    <t>PC=PC+1 || R1=0 || R30=C0 || R31=C1+C0 || R32=2*C1+C0 || R33=3*C1+C0 || R34=4*C1+C0 || R35=5*C1+C0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          PC=PC+1 || R3=0 || R30-=C0 || R31-=C0 || R32-=C0 || R33-=C0 || R34-=C0 || R35-=C0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        R3=R3+1 || PC=C15 || R30+=1 || R31+=1 || R32+=1 || R33+=1 || R34+=1 || R35+=1</t>
+  </si>
+  <si>
+    <t>R1=R1+1 || PC=C13 || R30+=C8 || R31+=C8 || R32+=C8 || R33+=C8 || R34+=C8 || R35+=C8</t>
+  </si>
+  <si>
+    <t>Nequ</t>
+  </si>
+  <si>
+    <t>C0 = C1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               PC=PC+1 || R5 = Mux(R4, R5, R3==0) || R6 = Mux(R4, R6, R3==1) || R7 = Mux(R4, R7, R3==2) ||  R8 = Mux(R4, R8, R3==3) ||  R9 = Mux(R4, R9, R3==4) || R10 = Mux(R4, R10, R3==5) || R20+=1 || R21+=1 || R22+=1 || R23+=1 || R24+=1 || R25+=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        PC = Mux(PC+1, PC+C12, R3&lt;C2) || A0Y=R1*C6+R2*C2+R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    PC=PC+1 || R4 = M0I*M0W + M1I*M1W + M2I*M2W + M3I*M3W + M4I*M4W + M5I*M5W || R11+=M0Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        R3=R3+1 || PC=C16 || R11 = R11-R5+R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    PC=PC+1 || V0Y=R11 || A0I = R20+=1 || A1I = R21+=1 || A2I = R22+=1 || A3I = R23+=1 || A4I = R24+=1 || A5I = R25+=1 || A0W   = R30 || A1W   = R31 || A2W   = R32 || A3W   = R33 || A4W   = R34 || A5W   = R35 || R5=R6|| R6=R7|| R7=R8|| R8=R9|| R9=R10|| R10=R4</t>
   </si>
 </sst>
 </file>
@@ -338,13 +327,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -642,38 +630,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="O26" zoomScale="132" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="14" max="14" width="7.26953125" customWidth="1"/>
-    <col min="15" max="15" width="181.81640625" customWidth="1"/>
+    <col min="15" max="15" width="255.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -684,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -695,7 +683,7 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -703,151 +691,154 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="I14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I18" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="I25" t="s">
+        <v>49</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -855,132 +846,174 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
       <c r="O27" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
         <v>6</v>
       </c>
-      <c r="O28" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N29">
+        <v>3</v>
+      </c>
       <c r="O29" s="3" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30">
-        <v>6</v>
-      </c>
-      <c r="C30">
-        <v>6</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
+      <c r="N30">
+        <v>4</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
+      <c r="N31">
+        <v>5</v>
       </c>
       <c r="O31" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N32">
+        <v>6</v>
+      </c>
       <c r="O32" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="15:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="O33" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="15:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="O34" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O35" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="15:15" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N33">
+        <v>7</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>8</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="N35">
+        <v>9</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N36">
+        <v>10</v>
+      </c>
       <c r="O36" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O37" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N37">
+        <v>11</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N38">
+        <v>12</v>
+      </c>
       <c r="O38" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="15:15" ht="43.5" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N39">
+        <v>13</v>
+      </c>
       <c r="O39" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O40" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N40">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="15:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="O41" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="15:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="O42" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O43" s="7" t="s">
+      <c r="O40" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N41">
+        <v>15</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N42">
+        <v>16</v>
+      </c>
+      <c r="O42" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O44" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O45" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O46" s="2" t="s">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N43">
         <v>17</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>